<commit_message>
added cGENIE folder with cGENIE files + implemented PO4_M in cGENIE
</commit_message>
<xml_diff>
--- a/Coversion_POC-flux.xlsx
+++ b/Coversion_POC-flux.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="211" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="211" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>I need core-top concentration of POC in mol cm-3 (or for interpretation wt%)</t>
   </si>
@@ -51,11 +51,11 @@
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
         <b val="true"/>
         <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">loc_new_sed_vol</t>
     </r>
@@ -103,10 +103,13 @@
     <t>CALCULATE SEDIMENT Corg concentration in mol cm-3</t>
   </si>
   <si>
-    <t>sed_calcCorg = loc_fPOC / [(1-dum_por) * loc_new_sed_vol]</t>
+    <t>sed_calcCorg =(1-dum_por) * loc_fPOC / loc_new_sed_vol</t>
   </si>
   <si>
     <t>mol/cm^3</t>
+  </si>
+  <si>
+    <t>!!!! Have to multiply (1-por), NOT devide!!!</t>
   </si>
   <si>
     <r>
@@ -114,10 +117,10 @@
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <sz val="10"/>
       </rPr>
       <t xml:space="preserve"> = mol cm-3 * g/mol * cm3/g</t>
     </r>
@@ -134,60 +137,60 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="0.00E+000" numFmtId="165"/>
-    <numFmt formatCode="0.00" numFmtId="166"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="0.00E+000"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
   <fonts count="8">
     <font>
-      <name val="Arial"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
-    </font>
-    <font>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
       <sz val="10"/>
-    </font>
-    <font>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
       <sz val="10"/>
-    </font>
-    <font>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="14"/>
-    </font>
-    <font>
-      <name val="Arial"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="12"/>
-    </font>
-    <font>
-      <name val="Arial"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <b val="true"/>
-      <color rgb="00FF0000"/>
-      <sz val="10"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -199,7 +202,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -208,51 +211,79 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="166" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="166" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -264,25 +295,26 @@
   </sheetPr>
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="B31" activeCellId="0" pane="topLeft" sqref="B31"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.6705882352941"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.7607843137255"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.4901960784314"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.2588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.6683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.7602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.4897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.7551020408163"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
         <v>1</v>
       </c>
@@ -290,7 +322,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -298,7 +330,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -312,7 +344,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
@@ -328,7 +360,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.25" outlineLevel="0" r="7">
+    <row r="7" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>9</v>
@@ -345,7 +377,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row r="8" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
@@ -369,7 +401,7 @@
         <v>0.173786</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row r="9" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
@@ -385,7 +417,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row r="10" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
@@ -401,7 +433,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
+    <row r="11" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
@@ -415,7 +447,7 @@
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    <row r="12" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="3" t="s">
         <v>17</v>
       </c>
@@ -429,17 +461,17 @@
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="13">
+    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    <row r="14" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
+    <row r="15" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
@@ -455,19 +487,19 @@
         <v>22</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
+    <row r="16" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
+    <row r="18" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="7" t="n">
         <f aca="false">(1-C11)*C15/(C7)</f>
-        <v>0.00572782084409991</v>
+        <v>0.00572782084409992</v>
       </c>
       <c r="D18" s="7" t="n">
         <f aca="false">(1-D11)*D15/(D7)</f>
@@ -476,16 +508,19 @@
       <c r="E18" s="0" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.25" outlineLevel="0" r="20">
+      <c r="F18" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C21" s="8" t="n">
         <f aca="false">100*C18*12/C12</f>
@@ -496,20 +531,20 @@
         <v>4.09710982658959</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
+    <row r="22" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C22" s="9" t="n">
         <f aca="false">100*C18*12/1</f>
-        <v>6.8733850129199</v>
+        <v>6.87338501291991</v>
       </c>
       <c r="D22" s="9" t="n">
         <f aca="false">100*D18*12/1</f>
         <v>10.242774566474</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+    <row r="24" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="n">
         <f aca="false">C8/C7*(1-C11)*1/12</f>
         <v>0.00572782084409991</v>
@@ -522,7 +557,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -537,17 +572,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7551020408163"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -562,17 +598,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7551020408163"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Matlab & Fortan: completed SWI-flux problem. LaTex: worked on reactions table and stiochiom. parameters
</commit_message>
<xml_diff>
--- a/Coversion_POC-flux.xlsx
+++ b/Coversion_POC-flux.xlsx
@@ -109,7 +109,7 @@
     <t>mol/cm^3</t>
   </si>
   <si>
-    <t>!!!! Have to multiply (1-por), NOT devide!!!</t>
+    <t>!!!! Have to multiply with (1-por), NOT divide!!!</t>
   </si>
   <si>
     <r>
@@ -296,7 +296,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
FORTRAN & matlab: SWI-flux: included advective flux at zinf also for other dissolved species like O2
</commit_message>
<xml_diff>
--- a/Coversion_POC-flux.xlsx
+++ b/Coversion_POC-flux.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>I need core-top concentration of POC in mol cm-3 (or for interpretation wt%)</t>
   </si>
@@ -126,6 +126,9 @@
     </r>
   </si>
   <si>
+    <t>HERE IS WHAT I, WHEN DIVIDE WITH (1-por):</t>
+  </si>
+  <si>
     <t>fun_sed_calcCorgwt = 100*fun_sed_calcCorg*12/dum_den</t>
   </si>
   <si>
@@ -141,7 +144,7 @@
     <numFmt numFmtId="165" formatCode="0.00E+000"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -188,6 +191,19 @@
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF800000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -235,7 +251,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -265,6 +281,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -293,10 +317,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -305,7 +329,9 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.7602040816327"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.4897959183673"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.7551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="11.7551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.9744897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -511,37 +537,64 @@
       <c r="F18" s="0" t="s">
         <v>26</v>
       </c>
+      <c r="I18" s="8" t="n">
+        <f aca="false">1/(1-C11)*C15/(C7)</f>
+        <v>0.143195521102498</v>
+      </c>
+      <c r="J18" s="8" t="n">
+        <f aca="false">1/(1-D11)*D15/(D7)</f>
+        <v>0.213391136801541</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="H20" s="9" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="8" t="n">
+        <v>29</v>
+      </c>
+      <c r="C21" s="10" t="n">
         <f aca="false">100*C18*12/C12</f>
         <v>2.74935400516796</v>
       </c>
-      <c r="D21" s="8" t="n">
+      <c r="D21" s="10" t="n">
         <f aca="false">100*D18*12/D12</f>
         <v>4.09710982658959</v>
       </c>
+      <c r="I21" s="10" t="n">
+        <f aca="false">100*I18*12/C12</f>
+        <v>68.7338501291991</v>
+      </c>
+      <c r="J21" s="10" t="n">
+        <f aca="false">100*J18*12/D12</f>
+        <v>102.42774566474</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="9" t="n">
+        <v>30</v>
+      </c>
+      <c r="C22" s="11" t="n">
         <f aca="false">100*C18*12/1</f>
         <v>6.87338501291991</v>
       </c>
-      <c r="D22" s="9" t="n">
+      <c r="D22" s="11" t="n">
         <f aca="false">100*D18*12/1</f>
         <v>10.242774566474</v>
+      </c>
+      <c r="I22" s="11" t="n">
+        <f aca="false">100*I18*12/1</f>
+        <v>171.834625322998</v>
+      </c>
+      <c r="J22" s="11" t="n">
+        <f aca="false">100*J18*12/1</f>
+        <v>256.06936416185</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>